<commit_message>
increased accuracy and precision
</commit_message>
<xml_diff>
--- a/movie_dataSet_2023.xlsx
+++ b/movie_dataSet_2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shett\OneDrive\Desktop\Project\ML mini-project\SharanShetty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shankar Prabhu S\Desktop\Movie-Verdict-Predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5122A84-F353-479F-B75D-2756032FB362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3BE04F-56EC-45E0-B5BD-76272E2B0E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2482,11 +2482,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F124" workbookViewId="0">
-      <selection activeCell="T141" sqref="T141"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140:X166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="24" width="19.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -7387,7 +7390,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="AB57" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.3">
@@ -8849,7 +8852,7 @@
         <v>5.2</v>
       </c>
       <c r="AB74" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
     </row>
     <row r="75" spans="1:28" x14ac:dyDescent="0.3">

</xml_diff>